<commit_message>
Update Leave Card 2/15/2023
</commit_message>
<xml_diff>
--- a/COSA, PAULA GRACE PANGANIBAN.xlsx
+++ b/COSA, PAULA GRACE PANGANIBAN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C984C2F7-CBD0-45CC-96B4-1FE7D08C72C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A701564D-54E3-4DD9-A79F-FEFAB91DCB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C4B9B69-0AD3-46D4-A495-D1BDE1D16EC6}"/>
   </bookViews>
@@ -29,20 +29,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>PERIOD</t>
   </si>
@@ -258,6 +250,9 @@
   </si>
   <si>
     <t>DOMESTIC 10/24/2022</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -1289,9 +1284,9 @@
   <dimension ref="A2:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3576" topLeftCell="A109" activePane="bottomLeft"/>
+      <pane ySplit="3576" topLeftCell="A112" activePane="bottomLeft"/>
       <selection activeCell="E9" sqref="E9"/>
-      <selection pane="bottomLeft" activeCell="K122" sqref="K122"/>
+      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,7 +1447,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>85.706000000000003</v>
+        <v>86.956000000000003</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -1462,7 +1457,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>40.707999999999998</v>
+        <v>41.957999999999998</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -3880,7 +3875,9 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="41"/>
+      <c r="A122" s="47" t="s">
+        <v>72</v>
+      </c>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
       <c r="D122" s="40"/>
@@ -3896,15 +3893,19 @@
       <c r="K122" s="20"/>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A123" s="41"/>
+      <c r="A123" s="41">
+        <v>44927</v>
+      </c>
       <c r="B123" s="20"/>
-      <c r="C123" s="13"/>
+      <c r="C123" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D123" s="40"/>
       <c r="E123" s="9"/>
       <c r="F123" s="20"/>
-      <c r="G123" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G123" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H123" s="40"/>
       <c r="I123" s="9"/>
@@ -3912,8 +3913,12 @@
       <c r="K123" s="20"/>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A124" s="41"/>
-      <c r="B124" s="20"/>
+      <c r="A124" s="41">
+        <v>44958</v>
+      </c>
+      <c r="B124" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="C124" s="13"/>
       <c r="D124" s="40"/>
       <c r="E124" s="9"/>
@@ -3925,7 +3930,9 @@
       <c r="H124" s="40"/>
       <c r="I124" s="9"/>
       <c r="J124" s="11"/>
-      <c r="K124" s="20"/>
+      <c r="K124" s="48">
+        <v>44957</v>
+      </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="41"/>

</xml_diff>